<commit_message>
Completed NearestNonMeetingMonth function! Huzzah!
</commit_message>
<xml_diff>
--- a/data/fomc_data.xlsx
+++ b/data/fomc_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackkidney/Documents/fedwatch/fedtool/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06C555D-007C-1547-8A2E-24CB65359315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C369DEF-5FB4-0F4A-88B6-C7186BCED8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23040" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -664,7 +664,7 @@
   <dimension ref="A1:G286"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2477,7 +2477,7 @@
         <v>0</v>
       </c>
       <c r="G82" s="4">
-        <f t="shared" ref="G82:G145" si="3">C82-D82</f>
+        <f t="shared" ref="G82:G138" si="3">C82-D82</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>